<commit_message>
Update BOM and Design with Digikey
</commit_message>
<xml_diff>
--- a/ESP32S3/ESP32S3 Master/BOM_esp32s3_master_2024-01-15.xlsx
+++ b/ESP32S3/ESP32S3 Master/BOM_esp32s3_master_2024-01-15.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="300">
   <si>
     <t>No.</t>
   </si>
@@ -658,33 +658,9 @@
     <t>23</t>
   </si>
   <si>
-    <t>TS-1928-B</t>
-  </si>
-  <si>
     <t>SW2</t>
   </si>
   <si>
-    <t>KEY-SMD_4P-L2.8-W2.0-P1.20-LS3.0-TL</t>
-  </si>
-  <si>
-    <t>XKB Connectivity(中国星坤)</t>
-  </si>
-  <si>
-    <t>C1121891</t>
-  </si>
-  <si>
-    <t>8615</t>
-  </si>
-  <si>
-    <t>0.1258</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
@@ -908,6 +884,36 @@
   </si>
   <si>
     <t>1965-ESP32-S3-MINI-1-N8TR-ND</t>
+  </si>
+  <si>
+    <t>2073-USB4105-GF-ATR-ND</t>
+  </si>
+  <si>
+    <t>SKSWCFE010</t>
+  </si>
+  <si>
+    <t>SW-SMD_L3.0-W2.0-LS3.5</t>
+  </si>
+  <si>
+    <t>ALPSALPINE(阿尔卑斯阿尔派)</t>
+  </si>
+  <si>
+    <t>C255576</t>
+  </si>
+  <si>
+    <t>23280</t>
+  </si>
+  <si>
+    <t>0.1470</t>
+  </si>
+  <si>
+    <t>15962</t>
+  </si>
+  <si>
+    <t>0.923</t>
+  </si>
+  <si>
+    <t>P123440TR-ND</t>
   </si>
 </sst>
 </file>
@@ -949,9 +955,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1276,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -1316,7 +1323,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -1363,7 +1370,7 @@
         <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="J3" t="s">
         <v>32</v>
@@ -1410,7 +1417,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="J4" t="s">
         <v>41</v>
@@ -1457,7 +1464,7 @@
         <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="J5" t="s">
         <v>49</v>
@@ -1504,7 +1511,7 @@
         <v>20</v>
       </c>
       <c r="I6" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J6" t="s">
         <v>58</v>
@@ -1551,7 +1558,7 @@
         <v>65</v>
       </c>
       <c r="I7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="J7" t="s">
         <v>66</v>
@@ -1598,7 +1605,7 @@
         <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="J8" t="s">
         <v>76</v>
@@ -1645,7 +1652,7 @@
         <v>85</v>
       </c>
       <c r="I9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="J9" t="s">
         <v>86</v>
@@ -1692,7 +1699,7 @@
         <v>93</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="J10" t="s">
         <v>94</v>
@@ -1739,7 +1746,7 @@
         <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="J11" t="s">
         <v>104</v>
@@ -1786,7 +1793,7 @@
         <v>113</v>
       </c>
       <c r="I12" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="J12" t="s">
         <v>114</v>
@@ -1833,7 +1840,7 @@
         <v>121</v>
       </c>
       <c r="I13" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="J13" t="s">
         <v>122</v>
@@ -1880,7 +1887,7 @@
         <v>131</v>
       </c>
       <c r="I14" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="J14" t="s">
         <v>132</v>
@@ -1927,7 +1934,7 @@
         <v>139</v>
       </c>
       <c r="I15" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="J15" t="s">
         <v>140</v>
@@ -1974,7 +1981,7 @@
         <v>148</v>
       </c>
       <c r="I16" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="J16" t="s">
         <v>149</v>
@@ -2021,7 +2028,7 @@
         <v>148</v>
       </c>
       <c r="I17" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="J17" t="s">
         <v>157</v>
@@ -2068,7 +2075,7 @@
         <v>148</v>
       </c>
       <c r="I18" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="J18" t="s">
         <v>165</v>
@@ -2115,7 +2122,7 @@
         <v>148</v>
       </c>
       <c r="I19" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="J19" t="s">
         <v>173</v>
@@ -2162,7 +2169,7 @@
         <v>148</v>
       </c>
       <c r="I20" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="J20" t="s">
         <v>182</v>
@@ -2209,7 +2216,7 @@
         <v>148</v>
       </c>
       <c r="I21" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="J21" t="s">
         <v>190</v>
@@ -2256,7 +2263,7 @@
         <v>198</v>
       </c>
       <c r="I22" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="J22" t="s">
         <v>199</v>
@@ -2303,7 +2310,7 @@
         <v>207</v>
       </c>
       <c r="I23" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="J23" t="s">
         <v>208</v>
@@ -2324,127 +2331,130 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>222</v>
+      <c r="E24" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" t="s">
+        <v>217</v>
+      </c>
+      <c r="E25" t="s">
+        <v>218</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" t="s">
+        <v>219</v>
+      </c>
+      <c r="I25" t="s">
+        <v>287</v>
+      </c>
+      <c r="J25" t="s">
+        <v>220</v>
+      </c>
+      <c r="K25" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" t="s">
+        <v>221</v>
+      </c>
+      <c r="M25" t="s">
+        <v>222</v>
+      </c>
+      <c r="N25" t="s">
+        <v>223</v>
+      </c>
+      <c r="O25" t="s">
         <v>224</v>
-      </c>
-      <c r="D25" t="s">
-        <v>225</v>
-      </c>
-      <c r="E25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" t="s">
-        <v>224</v>
-      </c>
-      <c r="H25" t="s">
-        <v>227</v>
-      </c>
-      <c r="I25" t="s">
-        <v>295</v>
-      </c>
-      <c r="J25" t="s">
-        <v>228</v>
-      </c>
-      <c r="K25" t="s">
-        <v>22</v>
-      </c>
-      <c r="L25" t="s">
-        <v>229</v>
-      </c>
-      <c r="M25" t="s">
-        <v>230</v>
-      </c>
-      <c r="N25" t="s">
-        <v>231</v>
-      </c>
-      <c r="O25" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D26" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E26" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F26" t="s">
         <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H26" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="I26" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J26" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K26" t="s">
         <v>22</v>
@@ -2456,145 +2466,148 @@
         <v>42</v>
       </c>
       <c r="N26" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="O26" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="C27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" t="s">
+        <v>234</v>
+      </c>
+      <c r="G27" t="s">
+        <v>237</v>
+      </c>
+      <c r="H27" t="s">
+        <v>238</v>
+      </c>
+      <c r="I27" t="s">
+        <v>289</v>
+      </c>
+      <c r="J27" t="s">
+        <v>239</v>
+      </c>
+      <c r="K27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" t="s">
+        <v>240</v>
+      </c>
+      <c r="M27" t="s">
+        <v>241</v>
+      </c>
+      <c r="N27" t="s">
         <v>242</v>
       </c>
-      <c r="D27" t="s">
+      <c r="O27" t="s">
         <v>243</v>
-      </c>
-      <c r="E27" t="s">
-        <v>244</v>
-      </c>
-      <c r="F27" t="s">
-        <v>242</v>
-      </c>
-      <c r="G27" t="s">
-        <v>245</v>
-      </c>
-      <c r="H27" t="s">
-        <v>246</v>
-      </c>
-      <c r="I27" t="s">
-        <v>297</v>
-      </c>
-      <c r="J27" t="s">
-        <v>247</v>
-      </c>
-      <c r="K27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" t="s">
-        <v>248</v>
-      </c>
-      <c r="M27" t="s">
-        <v>249</v>
-      </c>
-      <c r="N27" t="s">
-        <v>250</v>
-      </c>
-      <c r="O27" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="O28" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D28" s="1" t="s">
+    </row>
+    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L28" s="1" t="s">
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="I29" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="K29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="M29" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="N29" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="O29" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>